<commit_message>
Finishing up classification Appendix C
* Update RStudion to Version 1.4.984
</commit_message>
<xml_diff>
--- a/R/CH83-ClassificationTask/File3.xlsx
+++ b/R/CH83-ClassificationTask/File3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Dev/GitHub/RJafrocBook/R/CH83-ClassificationTask/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1819C21-6150-064D-B63C-4889F88442DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{405BFBB1-CE25-0A4A-8A4D-E4B32DAA9465}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12180" yWindow="7900" windowWidth="10000" windowHeight="8040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13060" yWindow="5300" windowWidth="10000" windowHeight="8040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TP" sheetId="1" r:id="rId1"/>
@@ -1833,7 +1833,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showRuler="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -2024,8 +2024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>